<commit_message>
day 3 finished - looking good
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -20,11 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="267">
   <si>
     <t xml:space="preserve">Data, Fresnell relations</t>
   </si>
   <si>
+    <t xml:space="preserve">DAY 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAY3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Measuring: </t>
   </si>
   <si>
@@ -64,6 +70,24 @@
     <t xml:space="preserve">RUN 7</t>
   </si>
   <si>
+    <t xml:space="preserve">RUN8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air-glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUN9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glass-air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUN10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUN11</t>
+  </si>
+  <si>
     <t xml:space="preserve">s or p:</t>
   </si>
   <si>
@@ -112,6 +136,24 @@
     <t xml:space="preserve">3.61</t>
   </si>
   <si>
+    <t xml:space="preserve">0.0537</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.25</t>
+  </si>
+  <si>
     <t xml:space="preserve">𝜃_1</t>
   </si>
   <si>
@@ -160,9 +202,6 @@
     <t xml:space="preserve">24</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0537</t>
-  </si>
-  <si>
     <t xml:space="preserve">23</t>
   </si>
   <si>
@@ -172,6 +211,18 @@
     <t xml:space="preserve">5</t>
   </si>
   <si>
+    <t xml:space="preserve">3.84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.59</t>
+  </si>
+  <si>
     <t xml:space="preserve">19</t>
   </si>
   <si>
@@ -220,6 +271,24 @@
     <t xml:space="preserve">11</t>
   </si>
   <si>
+    <t xml:space="preserve">3.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.42</t>
   </si>
   <si>
@@ -232,9 +301,6 @@
     <t xml:space="preserve">2.40</t>
   </si>
   <si>
-    <t xml:space="preserve">170</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.083</t>
   </si>
   <si>
@@ -268,6 +334,15 @@
     <t xml:space="preserve">14</t>
   </si>
   <si>
+    <t xml:space="preserve">3.78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">166.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.55</t>
+  </si>
+  <si>
     <t xml:space="preserve">40</t>
   </si>
   <si>
@@ -313,6 +388,21 @@
     <t xml:space="preserve">18</t>
   </si>
   <si>
+    <t xml:space="preserve">3.73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.48</t>
+  </si>
+  <si>
     <t xml:space="preserve">49</t>
   </si>
   <si>
@@ -322,9 +412,6 @@
     <t xml:space="preserve">1.92</t>
   </si>
   <si>
-    <t xml:space="preserve">166</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.0389</t>
   </si>
   <si>
@@ -346,6 +433,15 @@
     <t xml:space="preserve">1.68</t>
   </si>
   <si>
+    <t xml:space="preserve">3.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.31</t>
+  </si>
+  <si>
     <t xml:space="preserve">60</t>
   </si>
   <si>
@@ -388,6 +484,15 @@
     <t xml:space="preserve">1.32</t>
   </si>
   <si>
+    <t xml:space="preserve">3.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.27</t>
+  </si>
+  <si>
     <t xml:space="preserve">70</t>
   </si>
   <si>
@@ -430,6 +535,21 @@
     <t xml:space="preserve">37</t>
   </si>
   <si>
+    <t xml:space="preserve">3.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">143.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150</t>
+  </si>
+  <si>
     <t xml:space="preserve">80</t>
   </si>
   <si>
@@ -466,6 +586,15 @@
     <t xml:space="preserve">0.012</t>
   </si>
   <si>
+    <t xml:space="preserve">2.96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.77</t>
+  </si>
+  <si>
     <t xml:space="preserve">85</t>
   </si>
   <si>
@@ -502,6 +631,15 @@
     <t xml:space="preserve">Zero above</t>
   </si>
   <si>
+    <t xml:space="preserve">43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">138</t>
+  </si>
+  <si>
     <t xml:space="preserve">65</t>
   </si>
   <si>
@@ -529,6 +667,9 @@
     <t xml:space="preserve">114</t>
   </si>
   <si>
+    <t xml:space="preserve">DEAD</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.565</t>
   </si>
   <si>
@@ -577,9 +718,6 @@
     <t xml:space="preserve">2.18</t>
   </si>
   <si>
-    <t xml:space="preserve">163</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.21</t>
   </si>
   <si>
@@ -595,6 +733,15 @@
     <t xml:space="preserve">Polarizing angle</t>
   </si>
   <si>
+    <t xml:space="preserve">Intensity is drifting…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beam is broadening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T+R can sum to over 1, since I(0) is not a maximum</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sensor slit</t>
   </si>
   <si>
@@ -604,22 +751,43 @@
     <t xml:space="preserve">0.2 mm</t>
   </si>
   <si>
+    <t xml:space="preserve">Rectify by multiplying with a constant found from theory –</t>
+  </si>
+  <si>
     <t xml:space="preserve">Collimating slit 4</t>
   </si>
   <si>
     <t xml:space="preserve">Collimating slit</t>
   </si>
   <si>
+    <t xml:space="preserve">Much better signal with larger slit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> even though we are to estimate n2</t>
+  </si>
+  <si>
     <t xml:space="preserve">No secondary focus leans (just before detector)</t>
   </si>
   <si>
     <t xml:space="preserve">Secondary focus leans in place</t>
   </si>
   <si>
+    <t xml:space="preserve">1.0mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Or dividing by the maximum value near theoretical max</t>
+  </si>
+  <si>
     <t xml:space="preserve">Great uncertainty due to large collimater</t>
   </si>
   <si>
     <t xml:space="preserve">Beam spreads out when theta &gt; 80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collimating slit n 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beam broadening @ 60</t>
   </si>
   <si>
     <t xml:space="preserve">Beam gets widened a lot! </t>
@@ -747,7 +915,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -784,6 +952,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,13 +973,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC35"/>
+  <dimension ref="A1:AW35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="93" zoomScaleNormal="93" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="93" zoomScaleNormal="93" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE31" activeCellId="0" sqref="AE31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19140625" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.2"/>
   </cols>
@@ -816,296 +988,483 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F2" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>3</v>
-      </c>
       <c r="H3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="T3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="W3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="X3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC3" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AQ3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="AR3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="AS3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AU3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="AV3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="AW3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I4" s="2"/>
       <c r="K4" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="I5" s="2"/>
       <c r="K5" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="Q5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="T5" s="4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="Y5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AA5" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="AB5" s="4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AS5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AV5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AW5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AS7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="5" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="I8" s="4" t="n">
         <f aca="false">180-H8</f>
@@ -1113,142 +1472,232 @@
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="X8" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="AA8" s="4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="AB8" s="4" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="AC8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE8" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AF8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AR8" s="0" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="AS8" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="AU8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AV8" s="0" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="AW8" s="0" t="n">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="4" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="4" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="4" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="AB9" s="4" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM9" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN9" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ9" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="AR9" s="0" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="AS9" s="0" t="n">
+        <v>173.5</v>
+      </c>
+      <c r="AU9" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="AV9" s="0" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="AW9" s="0" t="n">
+        <v>173.5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5" t="n">
         <v>30</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="4" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="I10" s="4" t="n">
         <f aca="false">180-H10</f>
@@ -1256,71 +1705,116 @@
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="4" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="4" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="X10" s="4" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="AA10" s="4" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="AB10" s="4" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AC10" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+      <c r="AE10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF10" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK10" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AO10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AQ10" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AR10" s="0" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="AS10" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="AU10" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AV10" s="0" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="AW10" s="0" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="5" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="4" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="I11" s="4" t="n">
         <f aca="false">180-H11</f>
@@ -1328,71 +1822,116 @@
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="4" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="N11" s="6"/>
       <c r="O11" s="4" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="Q11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="W11" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="S11" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="W11" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="X11" s="4" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="AA11" s="4" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="AB11" s="4" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="AC11" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>121</v>
+      </c>
+      <c r="AE11" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF11" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG11" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="AI11" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ11" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AK11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AN11" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO11" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AQ11" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AR11" s="0" t="n">
+        <v>4.06</v>
+      </c>
+      <c r="AS11" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="AU11" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AV11" s="0" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="AW11" s="0" t="n">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="5" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="4" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="I12" s="4" t="n">
         <f aca="false">180-H12</f>
@@ -1400,29 +1939,29 @@
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="4" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="4" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="S12" s="0" t="n">
         <v>45</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="U12" s="0" t="n">
         <v>94</v>
@@ -1431,7 +1970,7 @@
         <v>35</v>
       </c>
       <c r="X12" s="7" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="Y12" s="0" t="n">
         <v>74</v>
@@ -1440,31 +1979,76 @@
         <v>35</v>
       </c>
       <c r="AB12" s="7" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="AC12" s="0" t="n">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE12" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="AF12" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG12" s="0" t="n">
+        <v>164</v>
+      </c>
+      <c r="AI12" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AJ12" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="AK12" s="0" t="n">
+        <v>158</v>
+      </c>
+      <c r="AM12" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AN12" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO12" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="AQ12" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AR12" s="0" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="AS12" s="0" t="n">
+        <v>166</v>
+      </c>
+      <c r="AU12" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="AV12" s="0" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="AW12" s="0" t="n">
+        <v>161.5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="5" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="4" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="I13" s="4" t="n">
         <f aca="false">180-H13</f>
@@ -1472,38 +2056,38 @@
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="4" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="4" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="W13" s="0" t="n">
         <v>37</v>
       </c>
       <c r="X13" s="7" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="Y13" s="0" t="n">
         <v>78</v>
@@ -1512,102 +2096,190 @@
         <v>37</v>
       </c>
       <c r="AB13" s="7" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="AC13" s="0" t="n">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE13" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="AF13" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG13" s="0" t="n">
+        <v>161.5</v>
+      </c>
+      <c r="AI13" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AJ13" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AK13" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="AM13" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AN13" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="AO13" s="0" t="n">
+        <v>158</v>
+      </c>
+      <c r="AQ13" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="AR13" s="0" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="AS13" s="0" t="n">
+        <v>164</v>
+      </c>
+      <c r="AU13" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="AV13" s="0" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="AW13" s="0" t="n">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="5" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="4" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="4" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="4" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>129</v>
+        <v>164</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="U14" s="4" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="X14" s="4" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="AB14" s="4" t="s">
-        <v>134</v>
+        <v>169</v>
       </c>
       <c r="AC14" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>170</v>
+      </c>
+      <c r="AE14" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF14" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG14" s="4"/>
+      <c r="AI14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ14" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AK14" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AM14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AN14" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="AO14" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="AQ14" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="AR14" s="0" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="AS14" s="0" t="n">
+        <v>161.5</v>
+      </c>
+      <c r="AU14" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="AV14" s="0" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="AW14" s="0" t="n">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="5" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="4" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="I15" s="4" t="n">
         <f aca="false">180-H15</f>
@@ -1615,29 +2287,29 @@
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="4" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>141</v>
+        <v>181</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>142</v>
+        <v>182</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="4" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="S15" s="0" t="n">
         <v>57</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="U15" s="0" t="n">
         <v>118</v>
@@ -1646,7 +2318,7 @@
         <v>45</v>
       </c>
       <c r="X15" s="7" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="Y15" s="0" t="n">
         <v>93</v>
@@ -1655,31 +2327,76 @@
         <v>41</v>
       </c>
       <c r="AB15" s="7" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="AC15" s="0" t="n">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="AG15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="AJ15" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="AK15" s="0" t="n">
+        <v>137</v>
+      </c>
+      <c r="AM15" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AN15" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="AO15" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="AQ15" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="AR15" s="0" t="n">
+        <v>4.21</v>
+      </c>
+      <c r="AS15" s="0" t="n">
+        <v>159</v>
+      </c>
+      <c r="AU15" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="AV15" s="0" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="AW15" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="5" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>149</v>
+        <v>192</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="4" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>151</v>
+        <v>194</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
       <c r="I16" s="4" t="n">
         <f aca="false">180-H16</f>
@@ -1687,61 +2404,94 @@
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="4" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>153</v>
+        <v>196</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="4" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>154</v>
+        <v>197</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>155</v>
+        <v>198</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>156</v>
+        <v>199</v>
       </c>
       <c r="U16" s="4" t="s">
-        <v>157</v>
+        <v>200</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="X16" s="4" t="s">
-        <v>158</v>
+        <v>201</v>
       </c>
       <c r="Y16" s="4" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="AA16" s="4"/>
       <c r="AB16" s="4" t="s">
-        <v>159</v>
+        <v>202</v>
       </c>
       <c r="AC16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="4"/>
+      <c r="AI16" s="4"/>
+      <c r="AJ16" s="4"/>
+      <c r="AK16" s="4"/>
+      <c r="AM16" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="AN16" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="AO16" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ16" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="AR16" s="0" t="n">
+        <v>4.09</v>
+      </c>
+      <c r="AS16" s="0" t="n">
+        <v>156</v>
+      </c>
+      <c r="AU16" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="AV16" s="0" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="AW16" s="0" t="n">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
       <c r="F17" s="4" t="s">
-        <v>160</v>
+        <v>206</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>161</v>
+        <v>207</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
       <c r="I17" s="4" t="n">
         <f aca="false">180-H17</f>
@@ -1749,66 +2499,99 @@
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="4" t="s">
-        <v>160</v>
+        <v>206</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>163</v>
+        <v>209</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="S17" s="4" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="T17" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="U17" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W17" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="U17" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="W17" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="X17" s="4" t="s">
-        <v>167</v>
+        <v>213</v>
       </c>
       <c r="Y17" s="4" t="s">
-        <v>168</v>
+        <v>214</v>
       </c>
       <c r="AA17" s="4"/>
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE17" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF17" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AG17" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AI17" s="4"/>
+      <c r="AJ17" s="4"/>
+      <c r="AK17" s="4"/>
+      <c r="AM17" s="4"/>
+      <c r="AN17" s="4"/>
+      <c r="AO17" s="4"/>
+      <c r="AQ17" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="AR17" s="0" t="n">
+        <v>3.98</v>
+      </c>
+      <c r="AS17" s="0" t="n">
+        <v>153</v>
+      </c>
+      <c r="AU17" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="AV17" s="0" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="AW17" s="0" t="n">
+        <v>141.5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
       <c r="F18" s="4" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>169</v>
+        <v>216</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>170</v>
+        <v>217</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>171</v>
+        <v>218</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="4" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>172</v>
+        <v>219</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>173</v>
+        <v>220</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="4"/>
@@ -1818,31 +2601,58 @@
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="W18" s="4" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="X18" s="4" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="Y18" s="4" t="s">
-        <v>174</v>
+        <v>221</v>
       </c>
       <c r="AA18" s="4"/>
       <c r="AB18" s="4"/>
       <c r="AC18" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="4"/>
+      <c r="AI18" s="4"/>
+      <c r="AJ18" s="4"/>
+      <c r="AK18" s="4"/>
+      <c r="AM18" s="4"/>
+      <c r="AN18" s="4"/>
+      <c r="AO18" s="4"/>
+      <c r="AQ18" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="AR18" s="0" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="AS18" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="AU18" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="AV18" s="0" t="n">
+        <v>0.688</v>
+      </c>
+      <c r="AW18" s="0" t="n">
+        <v>136.5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
       <c r="F19" s="4" t="s">
-        <v>175</v>
+        <v>222</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>176</v>
+        <v>223</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>177</v>
+        <v>224</v>
       </c>
       <c r="I19" s="4" t="n">
         <f aca="false">180-H19</f>
@@ -1850,13 +2660,13 @@
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="4" t="s">
-        <v>175</v>
+        <v>222</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>178</v>
+        <v>225</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>179</v>
+        <v>226</v>
       </c>
       <c r="N19" s="6"/>
       <c r="O19" s="4"/>
@@ -1866,31 +2676,58 @@
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="W19" s="4" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="X19" s="4" t="s">
-        <v>180</v>
+        <v>227</v>
       </c>
       <c r="Y19" s="4" t="s">
-        <v>181</v>
+        <v>228</v>
       </c>
       <c r="AA19" s="4"/>
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="4"/>
+      <c r="AG19" s="4"/>
+      <c r="AI19" s="4"/>
+      <c r="AJ19" s="4"/>
+      <c r="AK19" s="4"/>
+      <c r="AM19" s="4"/>
+      <c r="AN19" s="4"/>
+      <c r="AO19" s="4"/>
+      <c r="AQ19" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="AR19" s="0" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="AS19" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="AU19" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="AV19" s="0" t="n">
+        <v>0.307</v>
+      </c>
+      <c r="AW19" s="0" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="4" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>177</v>
+        <v>224</v>
       </c>
       <c r="I20" s="4" t="n">
         <f aca="false">180-H20</f>
@@ -1898,13 +2735,13 @@
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="4" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>183</v>
+        <v>230</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="N20" s="6"/>
       <c r="O20" s="4"/>
@@ -1914,19 +2751,37 @@
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="W20" s="4" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
       <c r="X20" s="4" t="s">
-        <v>184</v>
+        <v>231</v>
       </c>
       <c r="Y20" s="4" t="s">
-        <v>185</v>
+        <v>125</v>
       </c>
       <c r="AA20" s="4"/>
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="4"/>
+      <c r="AG20" s="4"/>
+      <c r="AI20" s="4"/>
+      <c r="AJ20" s="4"/>
+      <c r="AK20" s="4"/>
+      <c r="AM20" s="4"/>
+      <c r="AN20" s="4"/>
+      <c r="AO20" s="4"/>
+      <c r="AQ20" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="AR20" s="0" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="AS20" s="0" t="n">
+        <v>141.5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1940,13 +2795,13 @@
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="4" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>186</v>
+        <v>232</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>155</v>
+        <v>198</v>
       </c>
       <c r="N21" s="6"/>
       <c r="O21" s="4"/>
@@ -1961,8 +2816,26 @@
       <c r="AA21" s="4"/>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="4"/>
+      <c r="AG21" s="4"/>
+      <c r="AI21" s="4"/>
+      <c r="AJ21" s="4"/>
+      <c r="AK21" s="4"/>
+      <c r="AM21" s="4"/>
+      <c r="AN21" s="4"/>
+      <c r="AO21" s="4"/>
+      <c r="AQ21" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="AR21" s="0" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="AS21" s="0" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1976,13 +2849,13 @@
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="4" t="s">
-        <v>187</v>
+        <v>233</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>188</v>
+        <v>234</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="N22" s="6"/>
       <c r="O22" s="4"/>
@@ -1997,8 +2870,26 @@
       <c r="AA22" s="4"/>
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="4"/>
+      <c r="AG22" s="4"/>
+      <c r="AI22" s="4"/>
+      <c r="AJ22" s="4"/>
+      <c r="AK22" s="4"/>
+      <c r="AM22" s="4"/>
+      <c r="AN22" s="4"/>
+      <c r="AO22" s="4"/>
+      <c r="AQ22" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="AR22" s="0" t="n">
+        <v>0.558</v>
+      </c>
+      <c r="AS22" s="0" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2027,8 +2918,17 @@
       <c r="AA23" s="4"/>
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="4"/>
+      <c r="AG23" s="4"/>
+      <c r="AI23" s="4"/>
+      <c r="AJ23" s="4"/>
+      <c r="AK23" s="4"/>
+      <c r="AM23" s="4"/>
+      <c r="AN23" s="4"/>
+      <c r="AO23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -2058,186 +2958,217 @@
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F26" s="0" t="s">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>50</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="M26" s="0" t="n">
         <v>50</v>
       </c>
       <c r="O26" s="0" t="s">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="Q26" s="0" t="n">
         <v>40</v>
       </c>
       <c r="S26" s="0" t="s">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="U26" s="0" t="n">
         <v>40</v>
       </c>
       <c r="W26" s="0" t="s">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="Y26" s="0" t="n">
         <v>40</v>
       </c>
       <c r="AA26" s="0" t="s">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="AC26" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="AE26" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM26" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="AQ26" s="0" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="0" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>192</v>
+        <v>241</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>193</v>
+        <v>242</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
       <c r="Q27" s="8" t="s">
-        <v>193</v>
+        <v>242</v>
       </c>
       <c r="S27" s="0" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
       <c r="U27" s="8" t="s">
-        <v>193</v>
+        <v>242</v>
       </c>
       <c r="W27" s="0" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
       <c r="Y27" s="8" t="s">
-        <v>193</v>
+        <v>242</v>
       </c>
       <c r="AA27" s="0" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
       <c r="AC27" s="8" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>242</v>
+      </c>
+      <c r="AQ27" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F28" s="0" t="s">
-        <v>194</v>
+        <v>244</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="M28" s="0" t="n">
         <v>2</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="Q28" s="0" t="n">
         <v>2</v>
       </c>
       <c r="S28" s="0" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="U28" s="0" t="n">
         <v>2</v>
       </c>
       <c r="W28" s="0" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="Y28" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AA28" s="0" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="AC28" s="0" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE28" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="AQ28" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F29" s="0" t="s">
-        <v>196</v>
+        <v>248</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>197</v>
+        <v>249</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>197</v>
+        <v>249</v>
       </c>
       <c r="S29" s="0" t="s">
-        <v>197</v>
+        <v>249</v>
       </c>
       <c r="W29" s="0" t="s">
-        <v>197</v>
+        <v>249</v>
       </c>
       <c r="AA29" s="0" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>249</v>
+      </c>
+      <c r="AE29" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="AQ29" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F30" s="0" t="s">
-        <v>198</v>
+        <v>252</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>199</v>
+        <v>253</v>
+      </c>
+      <c r="AE30" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="AQ30" s="0" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F31" s="0" t="s">
-        <v>200</v>
+        <v>256</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>201</v>
+        <v>257</v>
       </c>
       <c r="S31" s="0" t="s">
-        <v>202</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F32" s="0" t="s">
-        <v>203</v>
+        <v>259</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>204</v>
+        <v>260</v>
       </c>
       <c r="S32" s="0" t="s">
-        <v>205</v>
+        <v>261</v>
       </c>
       <c r="AA32" s="0" t="s">
-        <v>206</v>
+        <v>262</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F33" s="0" t="s">
-        <v>207</v>
+        <v>263</v>
       </c>
       <c r="AA33" s="0" t="s">
-        <v>208</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S34" s="0" t="s">
-        <v>209</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S35" s="0" t="s">
-        <v>210</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prelim figs - -with different normalization to account for the fact that I(0) is not the intensity max on the transmission curve
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,17 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\Fysik\4. semester\exp-phys2\exphys2\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DB660A-3060-41F0-93B1-F7B04CD2D57A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -20,820 +34,827 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="267">
-  <si>
-    <t xml:space="preserve">Data, Fresnell relations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAY 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAY3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="270">
+  <si>
+    <t>Data, Fresnell relations</t>
+  </si>
+  <si>
+    <t>DAY 2</t>
+  </si>
+  <si>
+    <t>DAY3</t>
   </si>
   <si>
     <t xml:space="preserve">Measuring: </t>
   </si>
   <si>
-    <t xml:space="preserve">RUN 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">air --&gt; glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transmission</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUN 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUN 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">air--&gt; glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reflection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUN 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUN 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glass --&gt; air</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUN 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUN 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUN8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air-glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUN9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glass-air</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUN10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUN11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s or p:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I(B)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I(0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40.8 mV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.79 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.7 mV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.54 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00509</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0537</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">𝜃_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I (V)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">𝜃_d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">𝜃_d corrected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.158</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">173.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0957</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">170</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">172.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0192</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">166.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">168</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0550</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.635</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00742</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">166</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">163</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0389</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.448</t>
-  </si>
-  <si>
-    <t xml:space="preserve">101.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">164</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0236</t>
-  </si>
-  <si>
-    <t xml:space="preserve">92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.936</t>
-  </si>
-  <si>
-    <t xml:space="preserve">122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0225</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">161.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">102.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">142</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.145</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.528</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">143.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.438</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">159</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00689</t>
-  </si>
-  <si>
-    <t xml:space="preserve">112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.199</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.77</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0674</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zero above</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.464</t>
-  </si>
-  <si>
-    <t xml:space="preserve">138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.872</t>
-  </si>
-  <si>
-    <t xml:space="preserve">154</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0573</t>
-  </si>
-  <si>
-    <t xml:space="preserve">132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">143</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.565</t>
-  </si>
-  <si>
-    <t xml:space="preserve">151.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">149</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.536</t>
-  </si>
-  <si>
-    <t xml:space="preserve">152.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.91</t>
-  </si>
-  <si>
-    <t xml:space="preserve">144</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0575</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polarizing angle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intensity is drifting…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beam is broadening</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T+R can sum to over 1, since I(0) is not a maximum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sensor slit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1 mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2 mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rectify by multiplying with a constant found from theory –</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collimating slit 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collimating slit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Much better signal with larger slit</t>
+    <t>RUN 1</t>
+  </si>
+  <si>
+    <t>air --&gt; glass</t>
+  </si>
+  <si>
+    <t>Transmission</t>
+  </si>
+  <si>
+    <t>RUN 2</t>
+  </si>
+  <si>
+    <t>RUN 3</t>
+  </si>
+  <si>
+    <t>air--&gt; glass</t>
+  </si>
+  <si>
+    <t>Reflection</t>
+  </si>
+  <si>
+    <t>RUN 4</t>
+  </si>
+  <si>
+    <t>RUN 5</t>
+  </si>
+  <si>
+    <t>glass --&gt; air</t>
+  </si>
+  <si>
+    <t>RUN 6</t>
+  </si>
+  <si>
+    <t>RUN 7</t>
+  </si>
+  <si>
+    <t>RUN8</t>
+  </si>
+  <si>
+    <t>Air-glass</t>
+  </si>
+  <si>
+    <t>RUN9</t>
+  </si>
+  <si>
+    <t>Glass-air</t>
+  </si>
+  <si>
+    <t>RUN10</t>
+  </si>
+  <si>
+    <t>RUN11</t>
+  </si>
+  <si>
+    <t>s or p:</t>
+  </si>
+  <si>
+    <t>I(B)</t>
+  </si>
+  <si>
+    <t>I(0)</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>40.8 mV</t>
+  </si>
+  <si>
+    <t>3.79 V</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>11.7 mV</t>
+  </si>
+  <si>
+    <t>2.54 V</t>
+  </si>
+  <si>
+    <t>0.00509</t>
+  </si>
+  <si>
+    <t>3.62</t>
+  </si>
+  <si>
+    <t>4.29</t>
+  </si>
+  <si>
+    <t>3.53</t>
+  </si>
+  <si>
+    <t>0.0111</t>
+  </si>
+  <si>
+    <t>2.95</t>
+  </si>
+  <si>
+    <t>3.61</t>
+  </si>
+  <si>
+    <t>0.0537</t>
+  </si>
+  <si>
+    <t>3.67</t>
+  </si>
+  <si>
+    <t>3.52</t>
+  </si>
+  <si>
+    <t>3.57</t>
+  </si>
+  <si>
+    <t>4.02</t>
+  </si>
+  <si>
+    <t>4.25</t>
+  </si>
+  <si>
+    <t>𝜃_1</t>
+  </si>
+  <si>
+    <t>I (V)</t>
+  </si>
+  <si>
+    <t>𝜃_d</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>𝜃_d corrected</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>3.74</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>2.76</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>0.158</t>
+  </si>
+  <si>
+    <t>21.5</t>
+  </si>
+  <si>
+    <t>0.214</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>0.0887</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>3.71</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>3.84</t>
+  </si>
+  <si>
+    <t>3.58</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>3.59</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>3.54</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>2.17</t>
+  </si>
+  <si>
+    <t>173.5</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>0.125</t>
+  </si>
+  <si>
+    <t>41.5</t>
+  </si>
+  <si>
+    <t>0.216</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>0.0957</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>0.0254</t>
+  </si>
+  <si>
+    <t>3.16</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>3.80</t>
+  </si>
+  <si>
+    <t>3.47</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>3.45</t>
+  </si>
+  <si>
+    <t>172.5</t>
+  </si>
+  <si>
+    <t>3.42</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>2.40</t>
+  </si>
+  <si>
+    <t>0.083</t>
+  </si>
+  <si>
+    <t>61.5</t>
+  </si>
+  <si>
+    <t>0.222</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>0.140</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>0.0192</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>2.84</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>3.78</t>
+  </si>
+  <si>
+    <t>166.5</t>
+  </si>
+  <si>
+    <t>3.55</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>3.04</t>
+  </si>
+  <si>
+    <t>13.5</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>2.01</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>0.0550</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>0.252</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>0.635</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>0.00742</t>
+  </si>
+  <si>
+    <t>2.22</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>3.73</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>3.23</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>3.48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>2.70</t>
+  </si>
+  <si>
+    <t>1.92</t>
+  </si>
+  <si>
+    <t>0.0389</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>0.448</t>
+  </si>
+  <si>
+    <t>101.5</t>
+  </si>
+  <si>
+    <t>1.29</t>
+  </si>
+  <si>
+    <t>0.00678</t>
+  </si>
+  <si>
+    <t>1.68</t>
+  </si>
+  <si>
+    <t>3.75</t>
+  </si>
+  <si>
+    <t>3.05</t>
+  </si>
+  <si>
+    <t>3.31</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>1.98</t>
+  </si>
+  <si>
+    <t>23.5</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>1.84</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>0.0236</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>0.936</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>1.45</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>0.0225</t>
+  </si>
+  <si>
+    <t>1.32</t>
+  </si>
+  <si>
+    <t>3.66</t>
+  </si>
+  <si>
+    <t>2.48</t>
+  </si>
+  <si>
+    <t>3.27</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>1.47</t>
+  </si>
+  <si>
+    <t>161.5</t>
+  </si>
+  <si>
+    <t>18.5</t>
+  </si>
+  <si>
+    <t>102.5</t>
+  </si>
+  <si>
+    <t>1.62</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>1.58</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>0.145</t>
+  </si>
+  <si>
+    <t>0.528</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>3.60</t>
+  </si>
+  <si>
+    <t>1.30</t>
+  </si>
+  <si>
+    <t>143.5</t>
+  </si>
+  <si>
+    <t>2.79</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>0.438</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>1.31</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>0.00689</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>3.25</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>1.83</t>
+  </si>
+  <si>
+    <t>1.18</t>
+  </si>
+  <si>
+    <t>0.012</t>
+  </si>
+  <si>
+    <t>2.96</t>
+  </si>
+  <si>
+    <t>0.199</t>
+  </si>
+  <si>
+    <t>1.77</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>0.0674</t>
+  </si>
+  <si>
+    <t>46.5</t>
+  </si>
+  <si>
+    <t>1.15</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>0.0141</t>
+  </si>
+  <si>
+    <t>2.09</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>2.05</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>1.23</t>
+  </si>
+  <si>
+    <t>Zero above</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>0.464</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>0.872</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>0.0573</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>2.19</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>1.37</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>DEAD</t>
+  </si>
+  <si>
+    <t>0.565</t>
+  </si>
+  <si>
+    <t>151.5</t>
+  </si>
+  <si>
+    <t>28.5</t>
+  </si>
+  <si>
+    <t>0.175</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>0.320</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>0.536</t>
+  </si>
+  <si>
+    <t>152.5</t>
+  </si>
+  <si>
+    <t>1.91</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>0.0575</t>
+  </si>
+  <si>
+    <t>1.13</t>
+  </si>
+  <si>
+    <t>2.18</t>
+  </si>
+  <si>
+    <t>1.21</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>1.89</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>Polarizing angle</t>
+  </si>
+  <si>
+    <t>Intensity is drifting…</t>
+  </si>
+  <si>
+    <t>Beam is broadening</t>
+  </si>
+  <si>
+    <t>T+R can sum to over 1, since I(0) is not a maximum</t>
+  </si>
+  <si>
+    <t>Sensor slit</t>
+  </si>
+  <si>
+    <t>0.1 mm</t>
+  </si>
+  <si>
+    <t>0.2 mm</t>
+  </si>
+  <si>
+    <t>Rectify by multiplying with a constant found from theory –</t>
+  </si>
+  <si>
+    <t>Collimating slit 4</t>
+  </si>
+  <si>
+    <t>Collimating slit</t>
+  </si>
+  <si>
+    <t>Much better signal with larger slit</t>
   </si>
   <si>
     <t xml:space="preserve"> even though we are to estimate n2</t>
   </si>
   <si>
-    <t xml:space="preserve">No secondary focus leans (just before detector)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary focus leans in place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Or dividing by the maximum value near theoretical max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Great uncertainty due to large collimater</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beam spreads out when theta &gt; 80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collimating slit n 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beam broadening @ 60</t>
+    <t>No secondary focus leans (just before detector)</t>
+  </si>
+  <si>
+    <t>Secondary focus leans in place</t>
+  </si>
+  <si>
+    <t>1.0mm</t>
+  </si>
+  <si>
+    <t>Or dividing by the maximum value near theoretical max</t>
+  </si>
+  <si>
+    <t>Great uncertainty due to large collimater</t>
+  </si>
+  <si>
+    <t>Beam spreads out when theta &gt; 80</t>
+  </si>
+  <si>
+    <t>Collimating slit n 2</t>
+  </si>
+  <si>
+    <t>Beam broadening @ 60</t>
   </si>
   <si>
     <t xml:space="preserve">Beam gets widened a lot! </t>
   </si>
   <si>
-    <t xml:space="preserve">The last measurement might receive light</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weird internal reflection - beam broadening?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy spread across wider area: will mess up ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">which has not entered the dielectric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glass-&gt;air reflection haves the beam moving through 2x as much glass - scattering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intensity is definitely drifting…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The laser largely hit the back of the collimating slit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crazy sensitive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32.68 kSamples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 ms/div</t>
+    <t>The last measurement might receive light</t>
+  </si>
+  <si>
+    <t>Weird internal reflection - beam broadening?</t>
+  </si>
+  <si>
+    <t>Energy spread across wider area: will mess up ratio</t>
+  </si>
+  <si>
+    <t>which has not entered the dielectric</t>
+  </si>
+  <si>
+    <t>glass-&gt;air reflection haves the beam moving through 2x as much glass - scattering</t>
+  </si>
+  <si>
+    <t>Intensity is definitely drifting…</t>
+  </si>
+  <si>
+    <t>The laser largely hit the back of the collimating slit</t>
+  </si>
+  <si>
+    <t>Crazy sensitive</t>
+  </si>
+  <si>
+    <t>32.68 kSamples</t>
+  </si>
+  <si>
+    <t>20 ms/div</t>
+  </si>
+  <si>
+    <t>t_1</t>
+  </si>
+  <si>
+    <t>corr I</t>
+  </si>
+  <si>
+    <t>t_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="h:mm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -842,19 +863,24 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -866,251 +892,518 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="2">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AW35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AW52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="93" zoomScaleNormal="93" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE31" activeCellId="0" sqref="AE31"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="AL20" sqref="AL20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.2"/>
+    <col min="9" max="9" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F2" s="0" t="s">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="S3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="T3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="U3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="W3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="X3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="Y3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AA3" s="0" t="s">
+      <c r="AA3" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="0" t="s">
+      <c r="AB3" t="s">
         <v>13</v>
       </c>
-      <c r="AC3" s="0" t="s">
+      <c r="AC3" t="s">
         <v>6</v>
       </c>
-      <c r="AE3" s="0" t="s">
+      <c r="AE3" t="s">
         <v>16</v>
       </c>
-      <c r="AF3" s="0" t="s">
+      <c r="AF3" t="s">
         <v>17</v>
       </c>
-      <c r="AG3" s="0" t="s">
+      <c r="AG3" t="s">
         <v>6</v>
       </c>
-      <c r="AI3" s="0" t="s">
+      <c r="AI3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AJ3" s="0" t="s">
+      <c r="AJ3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AK3" s="0" t="s">
+      <c r="AK3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AM3" s="0" t="s">
+      <c r="AM3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AN3" s="0" t="s">
+      <c r="AN3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AO3" s="0" t="s">
+      <c r="AO3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AQ3" s="0" t="s">
+      <c r="AQ3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AR3" s="0" t="s">
+      <c r="AR3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AS3" s="0" t="s">
+      <c r="AS3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AU3" s="0" t="s">
+      <c r="AU3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AV3" s="0" t="s">
+      <c r="AV3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AW3" s="0" t="s">
+      <c r="AW3" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1221,7 +1514,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1332,8 +1625,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
@@ -1446,7 +1738,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>49</v>
       </c>
@@ -1466,8 +1758,8 @@
       <c r="H8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="4" t="n">
-        <f aca="false">180-H8</f>
+      <c r="I8" s="4">
+        <f>180-H8</f>
         <v>3</v>
       </c>
       <c r="J8" s="6"/>
@@ -1544,26 +1836,26 @@
       <c r="AO8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="AQ8" s="0" t="n">
+      <c r="AQ8">
         <v>10</v>
       </c>
-      <c r="AR8" s="0" t="n">
+      <c r="AR8">
         <v>4.01</v>
       </c>
-      <c r="AS8" s="0" t="n">
+      <c r="AS8">
         <v>177</v>
       </c>
-      <c r="AU8" s="0" t="n">
+      <c r="AU8">
         <v>10</v>
       </c>
-      <c r="AV8" s="0" t="n">
+      <c r="AV8">
         <v>4.25</v>
       </c>
-      <c r="AW8" s="0" t="n">
+      <c r="AW8">
         <v>177</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>67</v>
       </c>
@@ -1660,27 +1952,27 @@
       <c r="AO9" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="AQ9" s="0" t="n">
+      <c r="AQ9">
         <v>20</v>
       </c>
-      <c r="AR9" s="0" t="n">
+      <c r="AR9">
         <v>4.03</v>
       </c>
-      <c r="AS9" s="0" t="n">
+      <c r="AS9">
         <v>173.5</v>
       </c>
-      <c r="AU9" s="0" t="n">
+      <c r="AU9">
         <v>20</v>
       </c>
-      <c r="AV9" s="0" t="n">
-        <v>4.27</v>
-      </c>
-      <c r="AW9" s="0" t="n">
+      <c r="AV9">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="AW9">
         <v>173.5</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5" t="n">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
         <v>30</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1699,8 +1991,8 @@
       <c r="H10" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="I10" s="4" t="n">
-        <f aca="false">180-H10</f>
+      <c r="I10" s="4">
+        <f>180-H10</f>
         <v>10</v>
       </c>
       <c r="J10" s="6"/>
@@ -1777,26 +2069,26 @@
       <c r="AO10" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="AQ10" s="0" t="n">
+      <c r="AQ10">
         <v>30</v>
       </c>
-      <c r="AR10" s="0" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="AS10" s="0" t="n">
+      <c r="AR10">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="AS10">
         <v>170</v>
       </c>
-      <c r="AU10" s="0" t="n">
+      <c r="AU10">
         <v>30</v>
       </c>
-      <c r="AV10" s="0" t="n">
-        <v>4.23</v>
-      </c>
-      <c r="AW10" s="0" t="n">
+      <c r="AV10">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="AW10">
         <v>170</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>107</v>
       </c>
@@ -1816,8 +2108,8 @@
       <c r="H11" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="I11" s="4" t="n">
-        <f aca="false">180-H11</f>
+      <c r="I11" s="4">
+        <f>180-H11</f>
         <v>12</v>
       </c>
       <c r="J11" s="6"/>
@@ -1894,26 +2186,26 @@
       <c r="AO11" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AQ11" s="0" t="n">
+      <c r="AQ11">
         <v>35</v>
       </c>
-      <c r="AR11" s="0" t="n">
-        <v>4.06</v>
-      </c>
-      <c r="AS11" s="0" t="n">
+      <c r="AR11">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="AS11">
         <v>168</v>
       </c>
-      <c r="AU11" s="0" t="n">
+      <c r="AU11">
         <v>40</v>
       </c>
-      <c r="AV11" s="0" t="n">
+      <c r="AV11">
         <v>4.13</v>
       </c>
-      <c r="AW11" s="0" t="n">
+      <c r="AW11">
         <v>166</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>127</v>
       </c>
@@ -1933,8 +2225,8 @@
       <c r="H12" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="4" t="n">
-        <f aca="false">180-H12</f>
+      <c r="I12" s="4">
+        <f>180-H12</f>
         <v>14</v>
       </c>
       <c r="J12" s="6"/>
@@ -1957,80 +2249,80 @@
       <c r="Q12" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="S12" s="0" t="n">
+      <c r="S12">
         <v>45</v>
       </c>
       <c r="T12" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="U12" s="0" t="n">
+      <c r="U12">
         <v>94</v>
       </c>
-      <c r="W12" s="0" t="n">
+      <c r="W12">
         <v>35</v>
       </c>
       <c r="X12" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="Y12" s="0" t="n">
+      <c r="Y12">
         <v>74</v>
       </c>
-      <c r="AA12" s="0" t="n">
+      <c r="AA12">
         <v>35</v>
       </c>
       <c r="AB12" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="AC12" s="0" t="n">
+      <c r="AC12">
         <v>25</v>
       </c>
-      <c r="AE12" s="0" t="n">
+      <c r="AE12">
         <v>45</v>
       </c>
       <c r="AF12" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="AG12" s="0" t="n">
+      <c r="AG12">
         <v>164</v>
       </c>
-      <c r="AI12" s="0" t="n">
+      <c r="AI12">
         <v>35</v>
       </c>
       <c r="AJ12" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="AK12" s="0" t="n">
+      <c r="AK12">
         <v>158</v>
       </c>
-      <c r="AM12" s="0" t="n">
+      <c r="AM12">
         <v>30</v>
       </c>
       <c r="AN12" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="AO12" s="0" t="n">
+      <c r="AO12">
         <v>163</v>
       </c>
-      <c r="AQ12" s="0" t="n">
+      <c r="AQ12">
         <v>40</v>
       </c>
-      <c r="AR12" s="0" t="n">
+      <c r="AR12">
         <v>4.18</v>
       </c>
-      <c r="AS12" s="0" t="n">
+      <c r="AS12">
         <v>166</v>
       </c>
-      <c r="AU12" s="0" t="n">
+      <c r="AU12">
         <v>50</v>
       </c>
-      <c r="AV12" s="0" t="n">
+      <c r="AV12">
         <v>3.88</v>
       </c>
-      <c r="AW12" s="0" t="n">
+      <c r="AW12">
         <v>161.5</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>140</v>
       </c>
@@ -2050,8 +2342,8 @@
       <c r="H13" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="I13" s="4" t="n">
-        <f aca="false">180-H13</f>
+      <c r="I13" s="4">
+        <f>180-H13</f>
         <v>16</v>
       </c>
       <c r="J13" s="6"/>
@@ -2083,71 +2375,71 @@
       <c r="U13" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="W13" s="0" t="n">
+      <c r="W13">
         <v>37</v>
       </c>
       <c r="X13" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="Y13" s="0" t="n">
+      <c r="Y13">
         <v>78</v>
       </c>
-      <c r="AA13" s="0" t="n">
+      <c r="AA13">
         <v>37</v>
       </c>
       <c r="AB13" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="AC13" s="0" t="n">
+      <c r="AC13">
         <v>27</v>
       </c>
-      <c r="AE13" s="0" t="n">
+      <c r="AE13">
         <v>50</v>
       </c>
       <c r="AF13" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="AG13" s="0" t="n">
+      <c r="AG13">
         <v>161.5</v>
       </c>
-      <c r="AI13" s="0" t="n">
+      <c r="AI13">
         <v>40</v>
       </c>
       <c r="AJ13" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AK13" s="0" t="n">
+      <c r="AK13">
         <v>150</v>
       </c>
-      <c r="AM13" s="0" t="n">
+      <c r="AM13">
         <v>35</v>
       </c>
       <c r="AN13" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="AO13" s="0" t="n">
+      <c r="AO13">
         <v>158</v>
       </c>
-      <c r="AQ13" s="0" t="n">
+      <c r="AQ13">
         <v>45</v>
       </c>
-      <c r="AR13" s="0" t="n">
+      <c r="AR13">
         <v>4.26</v>
       </c>
-      <c r="AS13" s="0" t="n">
+      <c r="AS13">
         <v>164</v>
       </c>
-      <c r="AU13" s="0" t="n">
+      <c r="AU13">
         <v>60</v>
       </c>
-      <c r="AV13" s="0" t="n">
+      <c r="AV13">
         <v>3.44</v>
       </c>
-      <c r="AW13" s="0" t="n">
+      <c r="AW13">
         <v>156</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>157</v>
       </c>
@@ -2242,26 +2534,26 @@
       <c r="AO14" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="AQ14" s="0" t="n">
+      <c r="AQ14">
         <v>50</v>
       </c>
-      <c r="AR14" s="0" t="n">
-        <v>4.23</v>
-      </c>
-      <c r="AS14" s="0" t="n">
+      <c r="AR14">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="AS14">
         <v>161.5</v>
       </c>
-      <c r="AU14" s="0" t="n">
+      <c r="AU14">
         <v>65</v>
       </c>
-      <c r="AV14" s="0" t="n">
+      <c r="AV14">
         <v>3.2</v>
       </c>
-      <c r="AW14" s="0" t="n">
+      <c r="AW14">
         <v>153</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>176</v>
       </c>
@@ -2281,8 +2573,8 @@
       <c r="H15" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="I15" s="4" t="n">
-        <f aca="false">180-H15</f>
+      <c r="I15" s="4">
+        <f>180-H15</f>
         <v>21</v>
       </c>
       <c r="J15" s="6"/>
@@ -2305,80 +2597,80 @@
       <c r="Q15" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="S15" s="0" t="n">
+      <c r="S15">
         <v>57</v>
       </c>
       <c r="T15" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="U15" s="0" t="n">
+      <c r="U15">
         <v>118</v>
       </c>
-      <c r="W15" s="0" t="n">
+      <c r="W15">
         <v>45</v>
       </c>
       <c r="X15" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="Y15" s="0" t="n">
+      <c r="Y15">
         <v>93</v>
       </c>
-      <c r="AA15" s="0" t="n">
+      <c r="AA15">
         <v>41</v>
       </c>
       <c r="AB15" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="AC15" s="0" t="n">
+      <c r="AC15">
         <v>43</v>
       </c>
-      <c r="AE15" s="0" t="n">
+      <c r="AE15">
         <v>0</v>
       </c>
       <c r="AF15" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="AG15" s="0" t="n">
+      <c r="AG15">
         <v>0</v>
       </c>
-      <c r="AI15" s="0" t="n">
+      <c r="AI15">
         <v>43</v>
       </c>
       <c r="AJ15" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="AK15" s="0" t="n">
+      <c r="AK15">
         <v>137</v>
       </c>
-      <c r="AM15" s="0" t="n">
+      <c r="AM15">
         <v>42</v>
       </c>
       <c r="AN15" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="AO15" s="0" t="n">
+      <c r="AO15">
         <v>144</v>
       </c>
-      <c r="AQ15" s="0" t="n">
+      <c r="AQ15">
         <v>55</v>
       </c>
-      <c r="AR15" s="0" t="n">
+      <c r="AR15">
         <v>4.21</v>
       </c>
-      <c r="AS15" s="0" t="n">
+      <c r="AS15">
         <v>159</v>
       </c>
-      <c r="AU15" s="0" t="n">
+      <c r="AU15">
         <v>70</v>
       </c>
-      <c r="AV15" s="0" t="n">
+      <c r="AV15">
         <v>2.8</v>
       </c>
-      <c r="AW15" s="0" t="n">
+      <c r="AW15">
         <v>150</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>191</v>
       </c>
@@ -2398,8 +2690,8 @@
       <c r="H16" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="I16" s="4" t="n">
-        <f aca="false">180-H16</f>
+      <c r="I16" s="4">
+        <f>180-H16</f>
         <v>23</v>
       </c>
       <c r="J16" s="6"/>
@@ -2460,26 +2752,26 @@
       <c r="AO16" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="AQ16" s="0" t="n">
+      <c r="AQ16">
         <v>60</v>
       </c>
-      <c r="AR16" s="0" t="n">
+      <c r="AR16">
         <v>4.09</v>
       </c>
-      <c r="AS16" s="0" t="n">
+      <c r="AS16">
         <v>156</v>
       </c>
-      <c r="AU16" s="0" t="n">
+      <c r="AU16">
         <v>75</v>
       </c>
-      <c r="AV16" s="0" t="n">
+      <c r="AV16">
         <v>2.34</v>
       </c>
-      <c r="AW16" s="0" t="n">
+      <c r="AW16">
         <v>146</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -2493,8 +2785,8 @@
       <c r="H17" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="I17" s="4" t="n">
-        <f aca="false">180-H17</f>
+      <c r="I17" s="4">
+        <f>180-H17</f>
         <v>26</v>
       </c>
       <c r="J17" s="6"/>
@@ -2547,26 +2839,26 @@
       <c r="AM17" s="4"/>
       <c r="AN17" s="4"/>
       <c r="AO17" s="4"/>
-      <c r="AQ17" s="0" t="n">
+      <c r="AQ17">
         <v>65</v>
       </c>
-      <c r="AR17" s="0" t="n">
+      <c r="AR17">
         <v>3.98</v>
       </c>
-      <c r="AS17" s="0" t="n">
+      <c r="AS17">
         <v>153</v>
       </c>
-      <c r="AU17" s="0" t="n">
+      <c r="AU17">
         <v>80</v>
       </c>
-      <c r="AV17" s="0" t="n">
+      <c r="AV17">
         <v>1.69</v>
       </c>
-      <c r="AW17" s="0" t="n">
+      <c r="AW17">
         <v>141.5</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2621,26 +2913,26 @@
       <c r="AM18" s="4"/>
       <c r="AN18" s="4"/>
       <c r="AO18" s="4"/>
-      <c r="AQ18" s="0" t="n">
+      <c r="AQ18">
         <v>70</v>
       </c>
-      <c r="AR18" s="0" t="n">
+      <c r="AR18">
         <v>3.74</v>
       </c>
-      <c r="AS18" s="0" t="n">
+      <c r="AS18">
         <v>150</v>
       </c>
-      <c r="AU18" s="0" t="n">
+      <c r="AU18">
         <v>85</v>
       </c>
-      <c r="AV18" s="0" t="n">
-        <v>0.688</v>
-      </c>
-      <c r="AW18" s="0" t="n">
+      <c r="AV18">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="AW18">
         <v>136.5</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -2654,8 +2946,8 @@
       <c r="H19" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="I19" s="4" t="n">
-        <f aca="false">180-H19</f>
+      <c r="I19" s="4">
+        <f t="shared" ref="I19:I24" si="0">180-H19</f>
         <v>31</v>
       </c>
       <c r="J19" s="6"/>
@@ -2696,26 +2988,26 @@
       <c r="AM19" s="4"/>
       <c r="AN19" s="4"/>
       <c r="AO19" s="4"/>
-      <c r="AQ19" s="0" t="n">
+      <c r="AQ19">
         <v>75</v>
       </c>
-      <c r="AR19" s="0" t="n">
+      <c r="AR19">
         <v>3.39</v>
       </c>
-      <c r="AS19" s="0" t="n">
+      <c r="AS19">
         <v>146</v>
       </c>
-      <c r="AU19" s="0" t="n">
+      <c r="AU19">
         <v>87</v>
       </c>
-      <c r="AV19" s="0" t="n">
+      <c r="AV19">
         <v>0.307</v>
       </c>
-      <c r="AW19" s="0" t="n">
+      <c r="AW19">
         <v>134</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -2729,8 +3021,8 @@
       <c r="H20" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="I20" s="4" t="n">
-        <f aca="false">180-H20</f>
+      <c r="I20" s="4">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="J20" s="6"/>
@@ -2771,17 +3063,17 @@
       <c r="AM20" s="4"/>
       <c r="AN20" s="4"/>
       <c r="AO20" s="4"/>
-      <c r="AQ20" s="0" t="n">
+      <c r="AQ20">
         <v>80</v>
       </c>
-      <c r="AR20" s="0" t="n">
+      <c r="AR20">
         <v>2.71</v>
       </c>
-      <c r="AS20" s="0" t="n">
+      <c r="AS20">
         <v>141.5</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -2789,8 +3081,8 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="4" t="n">
-        <f aca="false">180-H21</f>
+      <c r="I21" s="4">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="J21" s="6"/>
@@ -2825,17 +3117,17 @@
       <c r="AM21" s="4"/>
       <c r="AN21" s="4"/>
       <c r="AO21" s="4"/>
-      <c r="AQ21" s="0" t="n">
+      <c r="AQ21">
         <v>85</v>
       </c>
-      <c r="AR21" s="0" t="n">
+      <c r="AR21">
         <v>1.47</v>
       </c>
-      <c r="AS21" s="0" t="n">
+      <c r="AS21">
         <v>136</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -2843,8 +3135,8 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="4" t="n">
-        <f aca="false">180-H22</f>
+      <c r="I22" s="4">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="J22" s="6"/>
@@ -2879,17 +3171,17 @@
       <c r="AM22" s="4"/>
       <c r="AN22" s="4"/>
       <c r="AO22" s="4"/>
-      <c r="AQ22" s="0" t="n">
+      <c r="AQ22">
         <v>87</v>
       </c>
-      <c r="AR22" s="0" t="n">
-        <v>0.558</v>
-      </c>
-      <c r="AS22" s="0" t="n">
+      <c r="AR22">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="AS22">
         <v>134</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2897,8 +3189,8 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="4" t="n">
-        <f aca="false">180-H23</f>
+      <c r="I23" s="4">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="J23" s="6"/>
@@ -2928,7 +3220,7 @@
       <c r="AN23" s="4"/>
       <c r="AO23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -2936,8 +3228,8 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="4" t="n">
-        <f aca="false">180-H24</f>
+      <c r="I24" s="4">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="J24" s="6"/>
@@ -2958,226 +3250,325 @@
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="0" t="s">
+    <row r="26" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
         <v>236</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26">
         <v>50</v>
       </c>
-      <c r="K26" s="0" t="s">
+      <c r="K26" t="s">
         <v>236</v>
       </c>
-      <c r="M26" s="0" t="n">
+      <c r="M26">
         <v>50</v>
       </c>
-      <c r="O26" s="0" t="s">
+      <c r="O26" t="s">
         <v>236</v>
       </c>
-      <c r="Q26" s="0" t="n">
+      <c r="Q26">
         <v>40</v>
       </c>
-      <c r="S26" s="0" t="s">
+      <c r="S26" t="s">
         <v>236</v>
       </c>
-      <c r="U26" s="0" t="n">
+      <c r="U26">
         <v>40</v>
       </c>
-      <c r="W26" s="0" t="s">
+      <c r="W26" t="s">
         <v>236</v>
       </c>
-      <c r="Y26" s="0" t="n">
+      <c r="Y26">
         <v>40</v>
       </c>
-      <c r="AA26" s="0" t="s">
+      <c r="AA26" t="s">
         <v>236</v>
       </c>
-      <c r="AC26" s="0" t="n">
+      <c r="AC26">
         <v>40</v>
       </c>
-      <c r="AE26" s="0" t="s">
+      <c r="AE26" t="s">
         <v>237</v>
       </c>
-      <c r="AM26" s="0" t="s">
+      <c r="AM26" t="s">
         <v>238</v>
       </c>
-      <c r="AQ26" s="0" t="s">
+      <c r="AQ26" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="0" t="s">
+    <row r="27" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
         <v>240</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="G27" t="s">
         <v>241</v>
       </c>
-      <c r="K27" s="0" t="s">
+      <c r="K27" t="s">
         <v>240</v>
       </c>
       <c r="M27" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="O27" s="0" t="s">
+      <c r="O27" t="s">
         <v>240</v>
       </c>
       <c r="Q27" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="S27" s="0" t="s">
+      <c r="S27" t="s">
         <v>240</v>
       </c>
       <c r="U27" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="W27" s="0" t="s">
+      <c r="W27" t="s">
         <v>240</v>
       </c>
       <c r="Y27" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="AA27" s="0" t="s">
+      <c r="AA27" t="s">
         <v>240</v>
       </c>
       <c r="AC27" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="AQ27" s="0" t="s">
+      <c r="AQ27" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="0" t="s">
+    <row r="28" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
         <v>244</v>
       </c>
-      <c r="K28" s="0" t="s">
+      <c r="K28" t="s">
         <v>245</v>
       </c>
-      <c r="M28" s="0" t="n">
+      <c r="M28">
         <v>2</v>
       </c>
-      <c r="O28" s="0" t="s">
+      <c r="O28" t="s">
         <v>245</v>
       </c>
-      <c r="Q28" s="0" t="n">
+      <c r="Q28">
         <v>2</v>
       </c>
-      <c r="S28" s="0" t="s">
+      <c r="S28" t="s">
         <v>245</v>
       </c>
-      <c r="U28" s="0" t="n">
+      <c r="U28">
         <v>2</v>
       </c>
-      <c r="W28" s="0" t="s">
+      <c r="W28" t="s">
         <v>245</v>
       </c>
-      <c r="Y28" s="0" t="n">
+      <c r="Y28">
         <v>2</v>
       </c>
-      <c r="AA28" s="0" t="s">
+      <c r="AA28" t="s">
         <v>245</v>
       </c>
-      <c r="AC28" s="0" t="n">
+      <c r="AC28">
         <v>2</v>
       </c>
-      <c r="AE28" s="0" t="s">
+      <c r="AE28" t="s">
         <v>246</v>
       </c>
       <c r="AQ28" s="9" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F29" s="0" t="s">
+    <row r="29" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
         <v>248</v>
       </c>
-      <c r="K29" s="0" t="s">
+      <c r="K29" t="s">
         <v>249</v>
       </c>
-      <c r="O29" s="0" t="s">
+      <c r="O29" t="s">
         <v>249</v>
       </c>
-      <c r="S29" s="0" t="s">
+      <c r="S29" t="s">
         <v>249</v>
       </c>
-      <c r="W29" s="0" t="s">
+      <c r="W29" t="s">
         <v>249</v>
       </c>
-      <c r="AA29" s="0" t="s">
+      <c r="AA29" t="s">
         <v>249</v>
       </c>
-      <c r="AE29" s="0" t="s">
+      <c r="AE29" t="s">
         <v>250</v>
       </c>
-      <c r="AQ29" s="0" t="s">
+      <c r="AQ29" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="0" t="s">
+    <row r="30" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
         <v>252</v>
       </c>
-      <c r="K30" s="0" t="s">
+      <c r="K30" t="s">
         <v>253</v>
       </c>
-      <c r="AE30" s="0" t="s">
+      <c r="AE30" t="s">
         <v>254</v>
       </c>
-      <c r="AQ30" s="0" t="s">
+      <c r="AQ30" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="0" t="s">
+    <row r="31" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
         <v>256</v>
       </c>
-      <c r="K31" s="0" t="s">
+      <c r="K31" t="s">
         <v>257</v>
       </c>
-      <c r="S31" s="0" t="s">
+      <c r="S31" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F32" s="0" t="s">
+    <row r="32" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
         <v>259</v>
       </c>
-      <c r="K32" s="0" t="s">
+      <c r="K32" t="s">
         <v>260</v>
       </c>
-      <c r="S32" s="0" t="s">
+      <c r="S32" t="s">
         <v>261</v>
       </c>
-      <c r="AA32" s="0" t="s">
+      <c r="AA32" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F33" s="0" t="s">
+    <row r="33" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
         <v>263</v>
       </c>
-      <c r="AA33" s="0" t="s">
+      <c r="AA33" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S34" s="0" t="s">
+    <row r="34" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="S34" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S35" s="0" t="s">
+    <row r="35" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="S35" t="s">
         <v>266</v>
       </c>
     </row>
+    <row r="37" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>267</v>
+      </c>
+      <c r="L37" t="s">
+        <v>268</v>
+      </c>
+      <c r="M37" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="38" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="K38" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L38" s="11" t="e">
+        <f>$L8-L5</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="39" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="K39" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L39" s="11"/>
+    </row>
+    <row r="40" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="K40" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L40" s="11"/>
+    </row>
+    <row r="41" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="K41" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L41" s="11"/>
+    </row>
+    <row r="42" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="K42" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L42" s="11"/>
+    </row>
+    <row r="43" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="K43" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L43" s="11"/>
+    </row>
+    <row r="44" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="K44" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="L44" s="11"/>
+    </row>
+    <row r="45" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="K45" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="L45" s="11"/>
+    </row>
+    <row r="46" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="K46" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="L46" s="11"/>
+    </row>
+    <row r="47" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="K47" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="L47" s="11"/>
+    </row>
+    <row r="48" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="K48" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="L48" s="11"/>
+    </row>
+    <row r="49" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K49" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="L49" s="11"/>
+    </row>
+    <row r="50" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K50" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="L50" s="11"/>
+    </row>
+    <row r="51" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K51" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="L51" s="11"/>
+    </row>
+    <row r="52" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K52" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="L52" s="11"/>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>